<commit_message>
Reshaped and renamed exploratory functions
</commit_message>
<xml_diff>
--- a/mediums/kwoji.xlsx
+++ b/mediums/kwoji.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentsrwthaachende-my.sharepoint.com/personal/ycy3t7jjvtr9b5h8_students_rwth-aachen_de/Documents/RWTH/Biotechnologie M. Sc/Masterarbeit/lmurinus_gem/mediums/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="956" documentId="11_AD4DB114E441178AC67DF4C8EED2F042693EDF13" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBF2882D-D4C8-4790-AAD1-AE36E0B2D8B9}"/>
+  <xr:revisionPtr revIDLastSave="1004" documentId="11_AD4DB114E441178AC67DF4C8EED2F042693EDF13" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F7A973B-4E37-4EDA-A328-B5EC2D93DDE6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="7140" windowWidth="21600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated media" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="222">
   <si>
     <t>Reaction</t>
   </si>
@@ -700,6 +700,9 @@
   </si>
   <si>
     <t>Folate</t>
+  </si>
+  <si>
+    <t>PO4H</t>
   </si>
 </sst>
 </file>
@@ -825,6 +828,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1255,14 +1266,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9E1F2"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1305,56 +1308,56 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7EDA9CF-183D-4DE6-B3F8-E34F47C7AFE5}" name="Table2" displayName="Table2" ref="A1:M77" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:M77" xr:uid="{D7EDA9CF-183D-4DE6-B3F8-E34F47C7AFE5}">
     <filterColumn colId="6">
-      <colorFilter dxfId="27"/>
+      <colorFilter dxfId="0"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A5161577-C6DE-4FE2-A90A-95510E158314}" name="Constituents" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{0D9E5566-C93E-42E3-8C64-9BA9A5DC796C}" name="Conc. in CDM (g/L)" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{1F245E0E-7450-4B0A-8688-83E97783477F}" name="Metabolite Name" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{6E393E52-8F40-4AF2-B3A0-DDFB7854F848}" name="Amount" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{3E410D9C-7FDE-4E3F-B523-727568B6AA69}" name="Present in Model" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{B535CB03-776B-4603-9A82-4B3EC8A74399}" name="e0 Metabolic ID" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{6E792D58-C946-44D6-9CEA-E19FBDE22A0F}" name="Exchange Reaction" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{CF071D84-8C1A-4342-A680-8E0D67E53882}" name="Ind. Conc." dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{A5161577-C6DE-4FE2-A90A-95510E158314}" name="Constituents" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{0D9E5566-C93E-42E3-8C64-9BA9A5DC796C}" name="Conc. in CDM (g/L)" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{1F245E0E-7450-4B0A-8688-83E97783477F}" name="Metabolite Name" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{6E393E52-8F40-4AF2-B3A0-DDFB7854F848}" name="Amount" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{3E410D9C-7FDE-4E3F-B523-727568B6AA69}" name="Present in Model" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{B535CB03-776B-4603-9A82-4B3EC8A74399}" name="e0 Metabolic ID" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{6E792D58-C946-44D6-9CEA-E19FBDE22A0F}" name="Exchange Reaction" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{CF071D84-8C1A-4342-A680-8E0D67E53882}" name="Ind. Conc." dataDxfId="20">
       <calculatedColumnFormula>Table2[[#This Row],[Conc. in CDM (g/L)]]*Table2[[#This Row],[Amount]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5F737F3F-E3DB-4DC3-B57B-49EE36EB379D}" name="Sum Conc." dataDxfId="18">
+    <tableColumn id="12" xr3:uid="{5F737F3F-E3DB-4DC3-B57B-49EE36EB379D}" name="Sum Conc." dataDxfId="19">
       <calculatedColumnFormula>IF(COUNTIF(G$2:G2,Table2[[#This Row],[Exchange Reaction]])=1,SUMIF(Table2[Exchange Reaction],Table2[[#This Row],[Exchange Reaction]],Table2[Ind. Conc.]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{89805C91-C2C4-4920-8591-8B9060035E82}" name="LB" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{8E714B77-51C6-4226-AB32-904D2C3421FC}" name="UB" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{922CA0D7-D586-46C3-B990-7266F8B342DF}" name="&quot;Dict&quot;" dataDxfId="15">
+    <tableColumn id="11" xr3:uid="{89805C91-C2C4-4920-8591-8B9060035E82}" name="LB" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{8E714B77-51C6-4226-AB32-904D2C3421FC}" name="UB" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{922CA0D7-D586-46C3-B990-7266F8B342DF}" name="&quot;Dict&quot;" dataDxfId="16">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Exchange Reaction]]="","",""""&amp;Table2[[#This Row],[Exchange Reaction]]&amp;"""")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F8CC4B19-B23C-4652-9068-972C12315475}" name="Bounds" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{F8CC4B19-B23C-4652-9068-972C12315475}" name="Bounds" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7756A3BD-E09F-46F5-B2AD-A111BFDD6735}" name="Table1" displayName="Table1" ref="A1:K48" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7756A3BD-E09F-46F5-B2AD-A111BFDD6735}" name="Table1" displayName="Table1" ref="A1:K48" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:K48" xr:uid="{7756A3BD-E09F-46F5-B2AD-A111BFDD6735}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K48">
     <sortCondition ref="A1:A48"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DF852FAD-8486-48B9-98B2-B7108DCDC05C}" name="Reaction" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{DF852FAD-8486-48B9-98B2-B7108DCDC05C}" name="Reaction" dataDxfId="12"/>
     <tableColumn id="11" xr3:uid="{DE0AE152-24CF-4498-8DB2-64AE1B31AC07}" name="For Python">
       <calculatedColumnFormula>""""&amp;Table1[[#This Row],[Reaction]]&amp;""""</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FDA76C6B-F149-4685-96A0-DFB159344365}" name="Met. ID" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{38FF68DF-27FE-4774-9F26-7410EFA8DAA6}" name="Met. Name" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{91ACCBDC-D7CA-4271-881D-951B09645297}" name="Component" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{BE8F368F-934D-4256-8357-FFF3B29E8FD9}" name="Type" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{4C8ACFFF-0D57-4C73-9CD7-0515E5EC627B}" name="Amount" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{10ED4E48-7E45-49C3-88FB-D3327B1F4C66}" name="Concentration" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{27E1AEC0-2088-4936-9EE1-1DFCD5FAF5C1}" name="LB" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{FDA76C6B-F149-4685-96A0-DFB159344365}" name="Met. ID" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{38FF68DF-27FE-4774-9F26-7410EFA8DAA6}" name="Met. Name" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{91ACCBDC-D7CA-4271-881D-951B09645297}" name="Component" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{BE8F368F-934D-4256-8357-FFF3B29E8FD9}" name="Type" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{4C8ACFFF-0D57-4C73-9CD7-0515E5EC627B}" name="Amount" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{10ED4E48-7E45-49C3-88FB-D3327B1F4C66}" name="Concentration" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{27E1AEC0-2088-4936-9EE1-1DFCD5FAF5C1}" name="LB" dataDxfId="5">
       <calculatedColumnFormula>(Table1[[#This Row],[Amount]]*Table1[[#This Row],[Concentration]])*-10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3AF485EB-A81E-4664-B596-DDC57A528545}" name="UB" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{1A8E6DAB-24D5-4F8F-BC4B-1A0029EF98E4}" name="Bounds" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{3AF485EB-A81E-4664-B596-DDC57A528545}" name="UB" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{1A8E6DAB-24D5-4F8F-BC4B-1A0029EF98E4}" name="Bounds" dataDxfId="3">
       <calculatedColumnFormula>"("&amp;Table1[[#This Row],[LB]]&amp;","&amp;Table1[[#This Row],[UB]]&amp;")"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1627,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794933BD-2EBE-4FDC-A981-C53C2BE8FFC4}">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M76"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,10 +1643,10 @@
     <col min="5" max="5" width="21" style="3" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" hidden="1" customWidth="1"/>
     <col min="9" max="10" width="14.28515625" style="3" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.140625" style="3" customWidth="1"/>
   </cols>
@@ -1745,7 +1748,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>221</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -4882,12 +4885,12 @@
     <row r="78" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="E2:E77">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G77">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>COUNTIF(G$2:G2,G2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
continued working on exploratory process document
</commit_message>
<xml_diff>
--- a/mediums/kwoji.xlsx
+++ b/mediums/kwoji.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentsrwthaachende-my.sharepoint.com/personal/ycy3t7jjvtr9b5h8_students_rwth-aachen_de/Documents/RWTH/Biotechnologie M. Sc/Masterarbeit/lmurinus_gem/mediums/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1004" documentId="11_AD4DB114E441178AC67DF4C8EED2F042693EDF13" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F7A973B-4E37-4EDA-A328-B5EC2D93DDE6}"/>
+  <xr:revisionPtr revIDLastSave="1008" documentId="11_AD4DB114E441178AC67DF4C8EED2F042693EDF13" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02C068B4-C8EF-47C5-BBC5-ECDC1DEC0F91}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="7140" windowWidth="21600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated media" sheetId="2" r:id="rId1"/>
@@ -828,14 +828,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9E1F2"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1266,6 +1258,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1308,56 +1308,56 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7EDA9CF-183D-4DE6-B3F8-E34F47C7AFE5}" name="Table2" displayName="Table2" ref="A1:M77" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:M77" xr:uid="{D7EDA9CF-183D-4DE6-B3F8-E34F47C7AFE5}">
     <filterColumn colId="6">
-      <colorFilter dxfId="0"/>
+      <colorFilter dxfId="27"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A5161577-C6DE-4FE2-A90A-95510E158314}" name="Constituents" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{0D9E5566-C93E-42E3-8C64-9BA9A5DC796C}" name="Conc. in CDM (g/L)" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{1F245E0E-7450-4B0A-8688-83E97783477F}" name="Metabolite Name" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{6E393E52-8F40-4AF2-B3A0-DDFB7854F848}" name="Amount" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{3E410D9C-7FDE-4E3F-B523-727568B6AA69}" name="Present in Model" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{B535CB03-776B-4603-9A82-4B3EC8A74399}" name="e0 Metabolic ID" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{6E792D58-C946-44D6-9CEA-E19FBDE22A0F}" name="Exchange Reaction" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{CF071D84-8C1A-4342-A680-8E0D67E53882}" name="Ind. Conc." dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{A5161577-C6DE-4FE2-A90A-95510E158314}" name="Constituents" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{0D9E5566-C93E-42E3-8C64-9BA9A5DC796C}" name="Conc. in CDM (g/L)" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{1F245E0E-7450-4B0A-8688-83E97783477F}" name="Metabolite Name" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{6E393E52-8F40-4AF2-B3A0-DDFB7854F848}" name="Amount" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{3E410D9C-7FDE-4E3F-B523-727568B6AA69}" name="Present in Model" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{B535CB03-776B-4603-9A82-4B3EC8A74399}" name="e0 Metabolic ID" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{6E792D58-C946-44D6-9CEA-E19FBDE22A0F}" name="Exchange Reaction" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{CF071D84-8C1A-4342-A680-8E0D67E53882}" name="Ind. Conc." dataDxfId="19">
       <calculatedColumnFormula>Table2[[#This Row],[Conc. in CDM (g/L)]]*Table2[[#This Row],[Amount]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5F737F3F-E3DB-4DC3-B57B-49EE36EB379D}" name="Sum Conc." dataDxfId="19">
+    <tableColumn id="12" xr3:uid="{5F737F3F-E3DB-4DC3-B57B-49EE36EB379D}" name="Sum Conc." dataDxfId="18">
       <calculatedColumnFormula>IF(COUNTIF(G$2:G2,Table2[[#This Row],[Exchange Reaction]])=1,SUMIF(Table2[Exchange Reaction],Table2[[#This Row],[Exchange Reaction]],Table2[Ind. Conc.]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{89805C91-C2C4-4920-8591-8B9060035E82}" name="LB" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{8E714B77-51C6-4226-AB32-904D2C3421FC}" name="UB" dataDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{922CA0D7-D586-46C3-B990-7266F8B342DF}" name="&quot;Dict&quot;" dataDxfId="16">
+    <tableColumn id="11" xr3:uid="{89805C91-C2C4-4920-8591-8B9060035E82}" name="LB" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{8E714B77-51C6-4226-AB32-904D2C3421FC}" name="UB" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{922CA0D7-D586-46C3-B990-7266F8B342DF}" name="&quot;Dict&quot;" dataDxfId="15">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Exchange Reaction]]="","",""""&amp;Table2[[#This Row],[Exchange Reaction]]&amp;"""")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F8CC4B19-B23C-4652-9068-972C12315475}" name="Bounds" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{F8CC4B19-B23C-4652-9068-972C12315475}" name="Bounds" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7756A3BD-E09F-46F5-B2AD-A111BFDD6735}" name="Table1" displayName="Table1" ref="A1:K48" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7756A3BD-E09F-46F5-B2AD-A111BFDD6735}" name="Table1" displayName="Table1" ref="A1:K48" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:K48" xr:uid="{7756A3BD-E09F-46F5-B2AD-A111BFDD6735}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K48">
     <sortCondition ref="A1:A48"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DF852FAD-8486-48B9-98B2-B7108DCDC05C}" name="Reaction" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{DF852FAD-8486-48B9-98B2-B7108DCDC05C}" name="Reaction" dataDxfId="11"/>
     <tableColumn id="11" xr3:uid="{DE0AE152-24CF-4498-8DB2-64AE1B31AC07}" name="For Python">
       <calculatedColumnFormula>""""&amp;Table1[[#This Row],[Reaction]]&amp;""""</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FDA76C6B-F149-4685-96A0-DFB159344365}" name="Met. ID" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{38FF68DF-27FE-4774-9F26-7410EFA8DAA6}" name="Met. Name" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{91ACCBDC-D7CA-4271-881D-951B09645297}" name="Component" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{BE8F368F-934D-4256-8357-FFF3B29E8FD9}" name="Type" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{4C8ACFFF-0D57-4C73-9CD7-0515E5EC627B}" name="Amount" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{10ED4E48-7E45-49C3-88FB-D3327B1F4C66}" name="Concentration" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{27E1AEC0-2088-4936-9EE1-1DFCD5FAF5C1}" name="LB" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{FDA76C6B-F149-4685-96A0-DFB159344365}" name="Met. ID" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{38FF68DF-27FE-4774-9F26-7410EFA8DAA6}" name="Met. Name" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{91ACCBDC-D7CA-4271-881D-951B09645297}" name="Component" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{BE8F368F-934D-4256-8357-FFF3B29E8FD9}" name="Type" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{4C8ACFFF-0D57-4C73-9CD7-0515E5EC627B}" name="Amount" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{10ED4E48-7E45-49C3-88FB-D3327B1F4C66}" name="Concentration" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{27E1AEC0-2088-4936-9EE1-1DFCD5FAF5C1}" name="LB" dataDxfId="4">
       <calculatedColumnFormula>(Table1[[#This Row],[Amount]]*Table1[[#This Row],[Concentration]])*-10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3AF485EB-A81E-4664-B596-DDC57A528545}" name="UB" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{1A8E6DAB-24D5-4F8F-BC4B-1A0029EF98E4}" name="Bounds" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{3AF485EB-A81E-4664-B596-DDC57A528545}" name="UB" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{1A8E6DAB-24D5-4F8F-BC4B-1A0029EF98E4}" name="Bounds" dataDxfId="2">
       <calculatedColumnFormula>"("&amp;Table1[[#This Row],[LB]]&amp;","&amp;Table1[[#This Row],[UB]]&amp;")"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794933BD-2EBE-4FDC-A981-C53C2BE8FFC4}">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4885,12 +4885,12 @@
     <row r="78" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="E2:E77">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G77">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(G$2:G2,G2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>